<commit_message>
commit dia antes del evento
</commit_message>
<xml_diff>
--- a/public/xls/FINALES.xlsx
+++ b/public/xls/FINALES.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="34220" yWindow="2280" windowWidth="28160" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="36440" yWindow="2200" windowWidth="28160" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="CLIENTES" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1977" uniqueCount="1202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2093" uniqueCount="1275">
   <si>
     <t>codigoBarras</t>
   </si>
@@ -3712,13 +3712,232 @@
   </si>
   <si>
     <t>anios</t>
+  </si>
+  <si>
+    <t>VIP0001</t>
+  </si>
+  <si>
+    <t>Karl P. Blank y Sra.</t>
+  </si>
+  <si>
+    <t>VIP0002</t>
+  </si>
+  <si>
+    <t>Mario Antonio Sandoval y Sra.</t>
+  </si>
+  <si>
+    <t>VIP0003</t>
+  </si>
+  <si>
+    <t>Jorge Tabarini y Sra.</t>
+  </si>
+  <si>
+    <t>VIP0004</t>
+  </si>
+  <si>
+    <t>Christian Blank y Sra.</t>
+  </si>
+  <si>
+    <t>VIP0005</t>
+  </si>
+  <si>
+    <t>Mario Alejandro Sandoval y Sra.</t>
+  </si>
+  <si>
+    <t>VIP0006</t>
+  </si>
+  <si>
+    <t>Felipe Izquierdo</t>
+  </si>
+  <si>
+    <t>VIP0007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Msc. </t>
+  </si>
+  <si>
+    <t>Miguel Ángel Méndez Zetina</t>
+  </si>
+  <si>
+    <t>Director Editorial</t>
+  </si>
+  <si>
+    <t>VIP0008</t>
+  </si>
+  <si>
+    <t>Jorge Estuardo Colindres Palacios</t>
+  </si>
+  <si>
+    <t>Gerente de Finanzas</t>
+  </si>
+  <si>
+    <t>VIP0009</t>
+  </si>
+  <si>
+    <t>Álvaro Noriega</t>
+  </si>
+  <si>
+    <t>VIP0010</t>
+  </si>
+  <si>
+    <t>Leonardo Rodríguez</t>
+  </si>
+  <si>
+    <t>Gerente de Planificación Digital</t>
+  </si>
+  <si>
+    <t>VIP0011</t>
+  </si>
+  <si>
+    <t>Lucrecia Choy Echeverría</t>
+  </si>
+  <si>
+    <t>Gerente de Desarrollo de Lector</t>
+  </si>
+  <si>
+    <t>VIP0012</t>
+  </si>
+  <si>
+    <t>Haroldo Sánchez</t>
+  </si>
+  <si>
+    <t>Director Noticiero Guatevisión</t>
+  </si>
+  <si>
+    <t>VIP0013</t>
+  </si>
+  <si>
+    <t>Ricardo García Santander</t>
+  </si>
+  <si>
+    <t>Gerente de Producción Guatevisión</t>
+  </si>
+  <si>
+    <t>VIP0014</t>
+  </si>
+  <si>
+    <t>Ricardo Asturias y Sra.</t>
+  </si>
+  <si>
+    <t>COL001</t>
+  </si>
+  <si>
+    <t>PRENSA LIBRE</t>
+  </si>
+  <si>
+    <t>GUATEVISION</t>
+  </si>
+  <si>
+    <t>Maria Luisa Gómez</t>
+  </si>
+  <si>
+    <t>Alejandro Vidal</t>
+  </si>
+  <si>
+    <t>Monica Moran</t>
+  </si>
+  <si>
+    <t>Sabrina Serrano</t>
+  </si>
+  <si>
+    <t>Andres Rosada</t>
+  </si>
+  <si>
+    <t>Jessica Solórzano</t>
+  </si>
+  <si>
+    <t>Jefe de Ventas</t>
+  </si>
+  <si>
+    <t>Territory Manager Cliente Directo</t>
+  </si>
+  <si>
+    <t>Territory Manager Digital</t>
+  </si>
+  <si>
+    <t>Territory Manager Agencias</t>
+  </si>
+  <si>
+    <t>COL002</t>
+  </si>
+  <si>
+    <t>COL003</t>
+  </si>
+  <si>
+    <t>COL004</t>
+  </si>
+  <si>
+    <t>COL005</t>
+  </si>
+  <si>
+    <t>COL006</t>
+  </si>
+  <si>
+    <t>COL007</t>
+  </si>
+  <si>
+    <t>COL008</t>
+  </si>
+  <si>
+    <t>Edwin Castañeda</t>
+  </si>
+  <si>
+    <t>Erick Santizo</t>
+  </si>
+  <si>
+    <t>COL009</t>
+  </si>
+  <si>
+    <t>COL010</t>
+  </si>
+  <si>
+    <t>COL011</t>
+  </si>
+  <si>
+    <t>COL012</t>
+  </si>
+  <si>
+    <t>Sara del Rosario Pacheco Ayala</t>
+  </si>
+  <si>
+    <t>Nancy Marisol Mendez Chacon</t>
+  </si>
+  <si>
+    <t>Brenda Rodríguez de Hernández</t>
+  </si>
+  <si>
+    <t>Badni Jesuá Sagastume</t>
+  </si>
+  <si>
+    <t>Conductor</t>
+  </si>
+  <si>
+    <t>Secretaria de Gerencia</t>
+  </si>
+  <si>
+    <t>Secretaria</t>
+  </si>
+  <si>
+    <t>Asistente Ejecutiva de Presidencia y Gerencia General</t>
+  </si>
+  <si>
+    <t>Analista Programador</t>
+  </si>
+  <si>
+    <t>Jefe de Frontoffice</t>
+  </si>
+  <si>
+    <t>VIP0015</t>
+  </si>
+  <si>
+    <t>Astrid Blank</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3726,8 +3945,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3746,6 +3972,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3759,10 +3997,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4051,10 +4293,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J235"/>
+  <dimension ref="A1:J262"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
+      <selection activeCell="F252" sqref="F252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11511,10 +11753,600 @@
         <v>1196</v>
       </c>
     </row>
+    <row r="236" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A236" s="3">
+        <v>2</v>
+      </c>
+      <c r="B236" s="3" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C236" s="3">
+        <v>20</v>
+      </c>
+      <c r="D236" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E236" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="F236" s="3" t="s">
+        <v>1203</v>
+      </c>
+      <c r="G236" s="3"/>
+      <c r="H236" s="3"/>
+    </row>
+    <row r="237" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A237" s="3">
+        <v>2</v>
+      </c>
+      <c r="B237" s="3" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C237" s="3">
+        <v>20</v>
+      </c>
+      <c r="D237" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E237" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="F237" s="3" t="s">
+        <v>1205</v>
+      </c>
+      <c r="G237" s="3"/>
+      <c r="H237" s="3"/>
+    </row>
+    <row r="238" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A238" s="3">
+        <v>2</v>
+      </c>
+      <c r="B238" s="3" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C238" s="3">
+        <v>20</v>
+      </c>
+      <c r="D238" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E238" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="F238" s="3" t="s">
+        <v>1207</v>
+      </c>
+      <c r="G238" s="3"/>
+      <c r="H238" s="3"/>
+    </row>
+    <row r="239" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A239" s="3">
+        <v>2</v>
+      </c>
+      <c r="B239" s="3" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C239" s="3">
+        <v>20</v>
+      </c>
+      <c r="D239" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E239" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="F239" s="3" t="s">
+        <v>1209</v>
+      </c>
+      <c r="G239" s="3"/>
+      <c r="H239" s="3"/>
+    </row>
+    <row r="240" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A240" s="3">
+        <v>2</v>
+      </c>
+      <c r="B240" s="3" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C240" s="3">
+        <v>20</v>
+      </c>
+      <c r="D240" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E240" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="F240" s="3" t="s">
+        <v>1211</v>
+      </c>
+      <c r="G240" s="3"/>
+      <c r="H240" s="3"/>
+    </row>
+    <row r="241" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A241" s="3">
+        <v>1</v>
+      </c>
+      <c r="B241" s="3" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C241" s="3">
+        <v>25</v>
+      </c>
+      <c r="D241" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E241" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="F241" s="3" t="s">
+        <v>1213</v>
+      </c>
+      <c r="G241" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="H241" s="3"/>
+    </row>
+    <row r="242" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A242" s="3">
+        <v>1</v>
+      </c>
+      <c r="B242" s="3" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C242" s="3">
+        <v>25</v>
+      </c>
+      <c r="D242" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E242" s="3" t="s">
+        <v>1215</v>
+      </c>
+      <c r="F242" s="3" t="s">
+        <v>1216</v>
+      </c>
+      <c r="G242" s="3" t="s">
+        <v>1217</v>
+      </c>
+      <c r="H242" s="3"/>
+    </row>
+    <row r="243" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A243" s="3">
+        <v>1</v>
+      </c>
+      <c r="B243" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C243" s="3">
+        <v>25</v>
+      </c>
+      <c r="D243" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E243" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="F243" s="3" t="s">
+        <v>1219</v>
+      </c>
+      <c r="G243" s="3" t="s">
+        <v>1220</v>
+      </c>
+      <c r="H243" s="3"/>
+    </row>
+    <row r="244" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A244" s="3">
+        <v>1</v>
+      </c>
+      <c r="B244" s="3" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C244" s="3">
+        <v>25</v>
+      </c>
+      <c r="D244" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E244" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="F244" s="3" t="s">
+        <v>1222</v>
+      </c>
+      <c r="G244" s="3" t="s">
+        <v>570</v>
+      </c>
+      <c r="H244" s="3"/>
+    </row>
+    <row r="245" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A245" s="3">
+        <v>1</v>
+      </c>
+      <c r="B245" s="3" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C245" s="3">
+        <v>25</v>
+      </c>
+      <c r="D245" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E245" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="F245" s="3" t="s">
+        <v>1224</v>
+      </c>
+      <c r="G245" s="3" t="s">
+        <v>1225</v>
+      </c>
+      <c r="H245" s="3"/>
+    </row>
+    <row r="246" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A246" s="3">
+        <v>1</v>
+      </c>
+      <c r="B246" s="3" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C246" s="3">
+        <v>25</v>
+      </c>
+      <c r="D246" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E246" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="F246" s="3" t="s">
+        <v>1227</v>
+      </c>
+      <c r="G246" s="3" t="s">
+        <v>1228</v>
+      </c>
+      <c r="H246" s="3"/>
+    </row>
+    <row r="247" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A247" s="3">
+        <v>1</v>
+      </c>
+      <c r="B247" s="3" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C247" s="3">
+        <v>25</v>
+      </c>
+      <c r="D247" s="3" t="s">
+        <v>1239</v>
+      </c>
+      <c r="E247" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="F247" s="3" t="s">
+        <v>1230</v>
+      </c>
+      <c r="G247" s="3" t="s">
+        <v>1231</v>
+      </c>
+      <c r="H247" s="3"/>
+    </row>
+    <row r="248" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A248" s="3">
+        <v>1</v>
+      </c>
+      <c r="B248" s="3" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C248" s="3">
+        <v>25</v>
+      </c>
+      <c r="D248" s="3" t="s">
+        <v>1239</v>
+      </c>
+      <c r="E248" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="F248" s="3" t="s">
+        <v>1233</v>
+      </c>
+      <c r="G248" s="3" t="s">
+        <v>1234</v>
+      </c>
+      <c r="H248" s="3"/>
+    </row>
+    <row r="249" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A249" s="3">
+        <v>2</v>
+      </c>
+      <c r="B249" s="3" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C249" s="3">
+        <v>25</v>
+      </c>
+      <c r="D249" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E249" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="F249" s="3" t="s">
+        <v>1236</v>
+      </c>
+      <c r="G249" s="3"/>
+      <c r="H249" s="3"/>
+    </row>
+    <row r="250" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A250" s="3">
+        <v>1</v>
+      </c>
+      <c r="B250" s="3" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C250" s="3">
+        <v>25</v>
+      </c>
+      <c r="D250" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E250" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="F250" s="3" t="s">
+        <v>1274</v>
+      </c>
+      <c r="G250" s="3"/>
+      <c r="H250" s="3"/>
+    </row>
+    <row r="251" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A251" s="5">
+        <v>1</v>
+      </c>
+      <c r="B251" s="5" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C251" s="5">
+        <v>25</v>
+      </c>
+      <c r="D251" s="5" t="s">
+        <v>1239</v>
+      </c>
+      <c r="E251" s="5"/>
+      <c r="F251" s="5" t="s">
+        <v>1240</v>
+      </c>
+      <c r="G251" s="6" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A252" s="5">
+        <v>1</v>
+      </c>
+      <c r="B252" s="5" t="s">
+        <v>1250</v>
+      </c>
+      <c r="C252" s="5">
+        <v>25</v>
+      </c>
+      <c r="D252" s="5" t="s">
+        <v>1239</v>
+      </c>
+      <c r="E252" s="5"/>
+      <c r="F252" s="5" t="s">
+        <v>1241</v>
+      </c>
+      <c r="G252" s="6" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A253" s="5">
+        <v>1</v>
+      </c>
+      <c r="B253" s="5" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C253" s="5">
+        <v>30</v>
+      </c>
+      <c r="D253" s="5" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E253" s="5"/>
+      <c r="F253" s="5" t="s">
+        <v>1263</v>
+      </c>
+      <c r="G253" s="6" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A254" s="5">
+        <v>1</v>
+      </c>
+      <c r="B254" s="5" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C254" s="5">
+        <v>30</v>
+      </c>
+      <c r="D254" s="5" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E254" s="5"/>
+      <c r="F254" s="5" t="s">
+        <v>1264</v>
+      </c>
+      <c r="G254" s="6" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A255" s="5">
+        <v>1</v>
+      </c>
+      <c r="B255" s="5" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C255" s="5">
+        <v>30</v>
+      </c>
+      <c r="D255" s="5" t="s">
+        <v>1238</v>
+      </c>
+      <c r="F255" s="5" t="s">
+        <v>1242</v>
+      </c>
+      <c r="G255" s="6" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A256" s="5">
+        <v>1</v>
+      </c>
+      <c r="B256" s="5" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C256" s="5">
+        <v>30</v>
+      </c>
+      <c r="D256" s="5" t="s">
+        <v>1238</v>
+      </c>
+      <c r="F256" s="5" t="s">
+        <v>1243</v>
+      </c>
+      <c r="G256" s="6" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A257" s="5">
+        <v>1</v>
+      </c>
+      <c r="B257" s="5" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C257" s="5">
+        <v>30</v>
+      </c>
+      <c r="D257" s="5" t="s">
+        <v>1238</v>
+      </c>
+      <c r="F257" s="5" t="s">
+        <v>1245</v>
+      </c>
+      <c r="G257" s="6" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A258" s="5">
+        <v>1</v>
+      </c>
+      <c r="B258" s="5" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C258" s="5">
+        <v>30</v>
+      </c>
+      <c r="D258" s="5" t="s">
+        <v>1238</v>
+      </c>
+      <c r="F258" s="5" t="s">
+        <v>1244</v>
+      </c>
+      <c r="G258" s="6" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="259" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A259" s="5">
+        <v>1</v>
+      </c>
+      <c r="B259" s="5" t="s">
+        <v>1259</v>
+      </c>
+      <c r="C259" s="5">
+        <v>30</v>
+      </c>
+      <c r="D259" s="5" t="s">
+        <v>1238</v>
+      </c>
+      <c r="F259" s="5" t="s">
+        <v>1265</v>
+      </c>
+      <c r="G259" s="6" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A260" s="5">
+        <v>1</v>
+      </c>
+      <c r="B260" s="5" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C260" s="5">
+        <v>30</v>
+      </c>
+      <c r="D260" s="5" t="s">
+        <v>1238</v>
+      </c>
+      <c r="F260" s="5" t="s">
+        <v>1266</v>
+      </c>
+      <c r="G260" s="6" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A261" s="5">
+        <v>1</v>
+      </c>
+      <c r="B261" s="5" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C261" s="5">
+        <v>30</v>
+      </c>
+      <c r="D261" s="5" t="s">
+        <v>1238</v>
+      </c>
+      <c r="F261" s="5" t="s">
+        <v>1257</v>
+      </c>
+      <c r="G261" s="6" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A262" s="5">
+        <v>1</v>
+      </c>
+      <c r="B262" s="5" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C262" s="5">
+        <v>30</v>
+      </c>
+      <c r="D262" s="5" t="s">
+        <v>1238</v>
+      </c>
+      <c r="F262" s="5" t="s">
+        <v>1258</v>
+      </c>
+      <c r="G262" s="6" t="s">
+        <v>1272</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>2</formula>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11526,7 +12358,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H18"/>
+      <selection activeCell="H3" sqref="H2:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>